<commit_message>
sub_plots in dashboard and minor improvments
</commit_message>
<xml_diff>
--- a/Marker_for_segments_v3.xlsx
+++ b/Marker_for_segments_v3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OLE_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OLE_APP_stable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3B7C0C-0186-4EE7-8E20-53A3092F9293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A4B6F1-899F-4FF3-82C4-4B3C0EE57064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HIP" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="FOOT" sheetId="4" r:id="rId4"/>
     <sheet name="MTP" sheetId="5" r:id="rId5"/>
     <sheet name="DISTAL_Marker" sheetId="6" r:id="rId6"/>
+    <sheet name="TORSO" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t>SIPS_right</t>
   </si>
@@ -249,6 +250,30 @@
   </si>
   <si>
     <t>L5MTP</t>
+  </si>
+  <si>
+    <t>C_7</t>
+  </si>
+  <si>
+    <t>B_10</t>
+  </si>
+  <si>
+    <t>sternum</t>
+  </si>
+  <si>
+    <t>clav</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>STERNUM</t>
+  </si>
+  <si>
+    <t>XYPHOID</t>
   </si>
 </sst>
 </file>
@@ -568,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -945,7 +970,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E3" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1037,4 +1062,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CD1CCC-83C6-4029-A1FE-E999CE91AF66}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>